<commit_message>
New function added, Now you can delete Data too.
</commit_message>
<xml_diff>
--- a/list_form.xlsx
+++ b/list_form.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5835" yWindow="3180" windowWidth="18300" windowHeight="10980" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="8805" yWindow="2955" windowWidth="18300" windowHeight="10980" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -412,10 +412,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:C9"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -431,81 +431,51 @@
     <row r="2">
       <c r="B2" t="inlineStr">
         <is>
-          <t>Fabio</t>
+          <t>Amareto</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>30</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="inlineStr">
         <is>
-          <t>Talita</t>
+          <t>Cleber</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="inlineStr">
         <is>
-          <t>Jose</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>34</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="inlineStr">
         <is>
-          <t>Amareto</t>
+          <t>Mary</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>52</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="inlineStr">
         <is>
-          <t>Zezinha</t>
+          <t>Peter</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Lucas</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Cleber</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Fabio</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>